<commit_message>
Added SSH authentication handling
</commit_message>
<xml_diff>
--- a/AP Config Sample Data.xlsx
+++ b/AP Config Sample Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">AP Name</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t xml:space="preserve">AP700F.6A54.1336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP1880.90E9.BE80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.19.4.145</t>
   </si>
 </sst>
 </file>
@@ -182,10 +188,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -299,7 +305,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>